<commit_message>
Tech Creator VBA FIX, new version
</commit_message>
<xml_diff>
--- a/Excel/14.02.2022 Stetson — техничка.xlsx
+++ b/Excel/14.02.2022 Stetson — техничка.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\BUH\ТЕХНИЧКИ\Stetson\Stetson_2022.02.08\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232F362E-E2A0-452F-8E9E-66EC5E032A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6546B932-7707-4F3B-B9DA-A1FC002EE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D646C5D-D16B-4A12-96BA-CB1DF5B2571A}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -640,9 +640,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2488,11 +2485,11 @@
   <sheetPr codeName="Лист10">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AN125"/>
+  <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ27" sqref="AJ27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="78" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2507,7 +2504,7 @@
     <col min="9" max="9" width="9" style="18"/>
     <col min="10" max="10" width="9" style="22"/>
     <col min="11" max="11" width="9" style="18"/>
-    <col min="12" max="12" width="15.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="28" bestFit="1" customWidth="1"/>
     <col min="13" max="22" width="9" style="18"/>
     <col min="23" max="23" width="9" style="18" customWidth="1"/>
     <col min="24" max="28" width="9" style="18"/>
@@ -2519,7 +2516,7 @@
     <col min="35" max="35" width="9.85546875" style="17" customWidth="1"/>
     <col min="36" max="37" width="10" style="17" customWidth="1"/>
     <col min="38" max="38" width="10.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7109375" style="32" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" style="31" customWidth="1"/>
     <col min="40" max="40" width="16.5703125" style="27" customWidth="1"/>
     <col min="41" max="16384" width="9" style="17"/>
   </cols>
@@ -2639,7 +2636,7 @@
       <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="30" t="s">
+      <c r="AM1" s="29" t="s">
         <v>129</v>
       </c>
       <c r="AN1" s="3" t="s">
@@ -2741,7 +2738,7 @@
       <c r="AL2" s="15">
         <v>2365.6880000000001</v>
       </c>
-      <c r="AM2" s="31">
+      <c r="AM2" s="30">
         <v>23.92</v>
       </c>
       <c r="AN2" s="16">
@@ -2843,7 +2840,7 @@
       <c r="AL3" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM3" s="31">
+      <c r="AM3" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN3" s="16">
@@ -2945,7 +2942,7 @@
       <c r="AL4" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM4" s="31">
+      <c r="AM4" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN4" s="16">
@@ -3047,7 +3044,7 @@
       <c r="AL5" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM5" s="31">
+      <c r="AM5" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN5" s="16">
@@ -3149,7 +3146,7 @@
       <c r="AL6" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM6" s="31">
+      <c r="AM6" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN6" s="16">
@@ -3251,7 +3248,7 @@
       <c r="AL7" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM7" s="31">
+      <c r="AM7" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN7" s="16">
@@ -3353,7 +3350,7 @@
       <c r="AL8" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM8" s="31">
+      <c r="AM8" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN8" s="16">
@@ -3455,7 +3452,7 @@
       <c r="AL9" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM9" s="31">
+      <c r="AM9" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN9" s="16">
@@ -3557,7 +3554,7 @@
       <c r="AL10" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM10" s="31">
+      <c r="AM10" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN10" s="16">
@@ -3659,7 +3656,7 @@
       <c r="AL11" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM11" s="31">
+      <c r="AM11" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN11" s="16">
@@ -3761,7 +3758,7 @@
       <c r="AL12" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM12" s="31">
+      <c r="AM12" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN12" s="16">
@@ -3863,7 +3860,7 @@
       <c r="AL13" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM13" s="31">
+      <c r="AM13" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN13" s="16">
@@ -3965,7 +3962,7 @@
       <c r="AL14" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM14" s="31">
+      <c r="AM14" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN14" s="16">
@@ -4067,7 +4064,7 @@
       <c r="AL15" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM15" s="31">
+      <c r="AM15" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN15" s="16">
@@ -4169,7 +4166,7 @@
       <c r="AL16" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM16" s="31">
+      <c r="AM16" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN16" s="16">
@@ -4271,7 +4268,7 @@
       <c r="AL17" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM17" s="31">
+      <c r="AM17" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN17" s="16">
@@ -4373,7 +4370,7 @@
       <c r="AL18" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM18" s="31">
+      <c r="AM18" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN18" s="16">
@@ -4475,7 +4472,7 @@
       <c r="AL19" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM19" s="31">
+      <c r="AM19" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN19" s="16">
@@ -4577,7 +4574,7 @@
       <c r="AL20" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM20" s="31">
+      <c r="AM20" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN20" s="16">
@@ -4679,7 +4676,7 @@
       <c r="AL21" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM21" s="31">
+      <c r="AM21" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN21" s="16">
@@ -4781,7 +4778,7 @@
       <c r="AL22" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM22" s="31">
+      <c r="AM22" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN22" s="16">
@@ -4883,7 +4880,7 @@
       <c r="AL23" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM23" s="31">
+      <c r="AM23" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN23" s="16">
@@ -4985,7 +4982,7 @@
       <c r="AL24" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM24" s="31">
+      <c r="AM24" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN24" s="16">
@@ -5087,7 +5084,7 @@
       <c r="AL25" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM25" s="31">
+      <c r="AM25" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN25" s="16">
@@ -5189,7 +5186,7 @@
       <c r="AL26" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM26" s="31">
+      <c r="AM26" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN26" s="16">
@@ -5291,7 +5288,7 @@
       <c r="AL27" s="15">
         <v>1178.8879999999997</v>
       </c>
-      <c r="AM27" s="31">
+      <c r="AM27" s="30">
         <v>11.920000000000002</v>
       </c>
       <c r="AN27" s="16">
@@ -5316,10 +5313,7 @@
       <c r="AJ28" s="17"/>
       <c r="AK28" s="17"/>
       <c r="AL28" s="26"/>
-      <c r="AM28" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN28" s="27"/>
+      <c r="AM28" s="27"/>
     </row>
     <row r="29" spans="1:40" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
@@ -5345,3820 +5339,11 @@
         <v>336.15000000000003</v>
       </c>
       <c r="AL29" s="26"/>
-      <c r="AM29" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN29" s="27"/>
-    </row>
-    <row r="30" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="D30" s="17"/>
-      <c r="F30" s="21"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="25"/>
-      <c r="AI30" s="17"/>
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
-      <c r="AL30" s="26"/>
-      <c r="AM30" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN30" s="27"/>
-    </row>
-    <row r="31" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="D31" s="17"/>
-      <c r="F31" s="21"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="17"/>
-      <c r="AD31" s="17"/>
-      <c r="AF31" s="17"/>
-      <c r="AG31" s="17"/>
-      <c r="AH31" s="25"/>
-      <c r="AI31" s="17"/>
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
-      <c r="AL31" s="26"/>
-      <c r="AM31" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN31" s="27"/>
-    </row>
-    <row r="32" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-      <c r="AH32" s="25"/>
-      <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
-      <c r="AL32" s="26"/>
-      <c r="AM32" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN32" s="27"/>
-    </row>
-    <row r="33" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="17"/>
-      <c r="AF33" s="17"/>
-      <c r="AG33" s="17"/>
-      <c r="AH33" s="25"/>
-      <c r="AI33" s="17"/>
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
-      <c r="AL33" s="26"/>
-      <c r="AM33" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN33" s="27"/>
-    </row>
-    <row r="34" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17"/>
-      <c r="AG34" s="17"/>
-      <c r="AH34" s="25"/>
-      <c r="AI34" s="17"/>
-      <c r="AJ34" s="17"/>
-      <c r="AK34" s="17"/>
-      <c r="AL34" s="26"/>
-      <c r="AM34" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN34" s="27"/>
-    </row>
-    <row r="35" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="17"/>
-      <c r="AH35" s="25"/>
-      <c r="AI35" s="17"/>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="26"/>
-      <c r="AM35" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN35" s="27"/>
-    </row>
-    <row r="36" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="AD36" s="17"/>
-      <c r="AE36" s="17"/>
-      <c r="AF36" s="17"/>
-      <c r="AG36" s="17"/>
-      <c r="AH36" s="25"/>
-      <c r="AI36" s="17"/>
-      <c r="AJ36" s="17"/>
-      <c r="AK36" s="17"/>
-      <c r="AL36" s="26"/>
-      <c r="AM36" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN36" s="27"/>
-    </row>
-    <row r="37" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="18"/>
-      <c r="Z37" s="18"/>
-      <c r="AA37" s="18"/>
-      <c r="AB37" s="18"/>
-      <c r="AC37" s="18"/>
-      <c r="AD37" s="17"/>
-      <c r="AE37" s="18"/>
-      <c r="AF37" s="17"/>
-      <c r="AG37" s="17"/>
-      <c r="AH37" s="25"/>
-      <c r="AI37" s="17"/>
-      <c r="AJ37" s="17"/>
-      <c r="AK37" s="17"/>
-      <c r="AL37" s="26"/>
-      <c r="AM37" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN37" s="27"/>
-    </row>
-    <row r="38" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="18"/>
-      <c r="Y38" s="18"/>
-      <c r="Z38" s="18"/>
-      <c r="AA38" s="18"/>
-      <c r="AB38" s="18"/>
-      <c r="AC38" s="18"/>
-      <c r="AD38" s="17"/>
-      <c r="AE38" s="18"/>
-      <c r="AF38" s="17"/>
-      <c r="AG38" s="17"/>
-      <c r="AH38" s="25"/>
-      <c r="AI38" s="17"/>
-      <c r="AJ38" s="17"/>
-      <c r="AK38" s="17"/>
-      <c r="AL38" s="26"/>
-      <c r="AM38" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN38" s="27"/>
-    </row>
-    <row r="39" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="18"/>
-      <c r="Z39" s="18"/>
-      <c r="AA39" s="18"/>
-      <c r="AB39" s="18"/>
-      <c r="AC39" s="18"/>
-      <c r="AD39" s="17"/>
-      <c r="AE39" s="18"/>
-      <c r="AF39" s="17"/>
-      <c r="AG39" s="17"/>
-      <c r="AH39" s="25"/>
-      <c r="AI39" s="17"/>
-      <c r="AJ39" s="17"/>
-      <c r="AK39" s="17"/>
-      <c r="AL39" s="26"/>
-      <c r="AM39" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN39" s="27"/>
-    </row>
-    <row r="40" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
-      <c r="Y40" s="18"/>
-      <c r="Z40" s="18"/>
-      <c r="AA40" s="18"/>
-      <c r="AB40" s="18"/>
-      <c r="AC40" s="18"/>
-      <c r="AD40" s="17"/>
-      <c r="AE40" s="18"/>
-      <c r="AF40" s="17"/>
-      <c r="AG40" s="17"/>
-      <c r="AH40" s="25"/>
-      <c r="AI40" s="17"/>
-      <c r="AJ40" s="17"/>
-      <c r="AK40" s="17"/>
-      <c r="AL40" s="26"/>
-      <c r="AM40" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN40" s="27"/>
-    </row>
-    <row r="41" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="18"/>
-      <c r="W41" s="18"/>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="18"/>
-      <c r="Z41" s="18"/>
-      <c r="AA41" s="18"/>
-      <c r="AB41" s="18"/>
-      <c r="AC41" s="18"/>
-      <c r="AD41" s="17"/>
-      <c r="AE41" s="18"/>
-      <c r="AF41" s="17"/>
-      <c r="AG41" s="17"/>
-      <c r="AH41" s="25"/>
-      <c r="AI41" s="17"/>
-      <c r="AJ41" s="17"/>
-      <c r="AK41" s="17"/>
-      <c r="AL41" s="26"/>
-      <c r="AM41" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN41" s="27"/>
-    </row>
-    <row r="42" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="18"/>
-      <c r="Z42" s="18"/>
-      <c r="AA42" s="18"/>
-      <c r="AB42" s="18"/>
-      <c r="AC42" s="18"/>
-      <c r="AD42" s="17"/>
-      <c r="AE42" s="18"/>
-      <c r="AF42" s="17"/>
-      <c r="AG42" s="17"/>
-      <c r="AH42" s="25"/>
-      <c r="AI42" s="17"/>
-      <c r="AJ42" s="17"/>
-      <c r="AK42" s="17"/>
-      <c r="AL42" s="26"/>
-      <c r="AM42" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN42" s="27"/>
-    </row>
-    <row r="43" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="18"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="18"/>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="18"/>
-      <c r="Z43" s="18"/>
-      <c r="AA43" s="18"/>
-      <c r="AB43" s="18"/>
-      <c r="AC43" s="18"/>
-      <c r="AD43" s="17"/>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="17"/>
-      <c r="AH43" s="25"/>
-      <c r="AI43" s="17"/>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-      <c r="AL43" s="26"/>
-      <c r="AM43" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN43" s="27"/>
-    </row>
-    <row r="44" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="18"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="18"/>
-      <c r="AA44" s="18"/>
-      <c r="AB44" s="18"/>
-      <c r="AC44" s="18"/>
-      <c r="AD44" s="17"/>
-      <c r="AE44" s="17"/>
-      <c r="AF44" s="17"/>
-      <c r="AG44" s="17"/>
-      <c r="AH44" s="25"/>
-      <c r="AI44" s="17"/>
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
-      <c r="AL44" s="26"/>
-      <c r="AM44" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN44" s="27"/>
-    </row>
-    <row r="45" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="18"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="18"/>
-      <c r="AA45" s="18"/>
-      <c r="AB45" s="18"/>
-      <c r="AC45" s="18"/>
-      <c r="AD45" s="17"/>
-      <c r="AE45" s="17"/>
-      <c r="AF45" s="17"/>
-      <c r="AG45" s="17"/>
-      <c r="AH45" s="25"/>
-      <c r="AI45" s="17"/>
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
-      <c r="AL45" s="26"/>
-      <c r="AM45" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN45" s="27"/>
-    </row>
-    <row r="46" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="18"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="18"/>
-      <c r="Z46" s="18"/>
-      <c r="AA46" s="18"/>
-      <c r="AB46" s="18"/>
-      <c r="AC46" s="18"/>
-      <c r="AD46" s="17"/>
-      <c r="AE46" s="17"/>
-      <c r="AF46" s="17"/>
-      <c r="AG46" s="17"/>
-      <c r="AH46" s="25"/>
-      <c r="AI46" s="17"/>
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
-      <c r="AL46" s="26"/>
-      <c r="AM46" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN46" s="27"/>
-    </row>
-    <row r="47" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="18"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
-      <c r="W47" s="18"/>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="18"/>
-      <c r="AA47" s="18"/>
-      <c r="AB47" s="18"/>
-      <c r="AC47" s="18"/>
-      <c r="AD47" s="17"/>
-      <c r="AE47" s="17"/>
-      <c r="AF47" s="17"/>
-      <c r="AG47" s="17"/>
-      <c r="AH47" s="25"/>
-      <c r="AI47" s="17"/>
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
-      <c r="AL47" s="26"/>
-      <c r="AM47" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN47" s="27"/>
-    </row>
-    <row r="48" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="18"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="U48" s="18"/>
-      <c r="V48" s="18"/>
-      <c r="W48" s="18"/>
-      <c r="X48" s="18"/>
-      <c r="Y48" s="18"/>
-      <c r="Z48" s="18"/>
-      <c r="AA48" s="18"/>
-      <c r="AB48" s="18"/>
-      <c r="AC48" s="18"/>
-      <c r="AD48" s="17"/>
-      <c r="AE48" s="17"/>
-      <c r="AF48" s="17"/>
-      <c r="AG48" s="17"/>
-      <c r="AH48" s="25"/>
-      <c r="AI48" s="17"/>
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
-      <c r="AL48" s="26"/>
-      <c r="AM48" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN48" s="27"/>
-    </row>
-    <row r="49" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="U49" s="18"/>
-      <c r="V49" s="18"/>
-      <c r="W49" s="18"/>
-      <c r="X49" s="18"/>
-      <c r="Y49" s="18"/>
-      <c r="Z49" s="18"/>
-      <c r="AA49" s="18"/>
-      <c r="AB49" s="18"/>
-      <c r="AC49" s="18"/>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="18"/>
-      <c r="AF49" s="17"/>
-      <c r="AG49" s="17"/>
-      <c r="AH49" s="25"/>
-      <c r="AI49" s="17"/>
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
-      <c r="AL49" s="26"/>
-      <c r="AM49" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN49" s="27"/>
-    </row>
-    <row r="50" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="18"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="18"/>
-      <c r="X50" s="18"/>
-      <c r="Y50" s="18"/>
-      <c r="Z50" s="18"/>
-      <c r="AA50" s="18"/>
-      <c r="AB50" s="18"/>
-      <c r="AC50" s="18"/>
-      <c r="AD50" s="17"/>
-      <c r="AE50" s="17"/>
-      <c r="AF50" s="17"/>
-      <c r="AG50" s="17"/>
-      <c r="AH50" s="25"/>
-      <c r="AI50" s="17"/>
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
-      <c r="AL50" s="26"/>
-      <c r="AM50" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN50" s="27"/>
-    </row>
-    <row r="51" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="23"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
-      <c r="V51" s="18"/>
-      <c r="W51" s="18"/>
-      <c r="X51" s="18"/>
-      <c r="Y51" s="18"/>
-      <c r="Z51" s="18"/>
-      <c r="AA51" s="18"/>
-      <c r="AB51" s="18"/>
-      <c r="AC51" s="18"/>
-      <c r="AD51" s="17"/>
-      <c r="AE51" s="18"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="17"/>
-      <c r="AH51" s="25"/>
-      <c r="AI51" s="17"/>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-      <c r="AL51" s="26"/>
-      <c r="AM51" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN51" s="27"/>
-    </row>
-    <row r="52" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="18"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="17"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
-      <c r="V52" s="18"/>
-      <c r="W52" s="18"/>
-      <c r="X52" s="18"/>
-      <c r="Y52" s="18"/>
-      <c r="Z52" s="18"/>
-      <c r="AA52" s="18"/>
-      <c r="AB52" s="18"/>
-      <c r="AC52" s="18"/>
-      <c r="AD52" s="17"/>
-      <c r="AE52" s="17"/>
-      <c r="AF52" s="17"/>
-      <c r="AG52" s="17"/>
-      <c r="AH52" s="25"/>
-      <c r="AI52" s="17"/>
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
-      <c r="AL52" s="26"/>
-      <c r="AM52" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN52" s="27"/>
-    </row>
-    <row r="53" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="18"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="17"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="17"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
-      <c r="V53" s="18"/>
-      <c r="W53" s="18"/>
-      <c r="X53" s="18"/>
-      <c r="Y53" s="18"/>
-      <c r="Z53" s="18"/>
-      <c r="AA53" s="18"/>
-      <c r="AB53" s="18"/>
-      <c r="AC53" s="18"/>
-      <c r="AD53" s="17"/>
-      <c r="AE53" s="17"/>
-      <c r="AF53" s="17"/>
-      <c r="AG53" s="17"/>
-      <c r="AH53" s="25"/>
-      <c r="AI53" s="17"/>
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
-      <c r="AL53" s="26"/>
-      <c r="AM53" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN53" s="27"/>
-    </row>
-    <row r="54" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="18"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-      <c r="U54" s="18"/>
-      <c r="V54" s="18"/>
-      <c r="W54" s="18"/>
-      <c r="X54" s="18"/>
-      <c r="Y54" s="18"/>
-      <c r="Z54" s="18"/>
-      <c r="AA54" s="18"/>
-      <c r="AB54" s="18"/>
-      <c r="AC54" s="18"/>
-      <c r="AD54" s="17"/>
-      <c r="AE54" s="17"/>
-      <c r="AF54" s="17"/>
-      <c r="AG54" s="17"/>
-      <c r="AH54" s="25"/>
-      <c r="AI54" s="17"/>
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
-      <c r="AL54" s="26"/>
-      <c r="AM54" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN54" s="27"/>
-    </row>
-    <row r="55" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="18"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="28"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="18"/>
-      <c r="U55" s="18"/>
-      <c r="V55" s="18"/>
-      <c r="W55" s="18"/>
-      <c r="X55" s="18"/>
-      <c r="Y55" s="18"/>
-      <c r="Z55" s="18"/>
-      <c r="AA55" s="18"/>
-      <c r="AB55" s="18"/>
-      <c r="AC55" s="18"/>
-      <c r="AD55" s="17"/>
-      <c r="AE55" s="17"/>
-      <c r="AF55" s="17"/>
-      <c r="AG55" s="17"/>
-      <c r="AH55" s="25"/>
-      <c r="AI55" s="17"/>
-      <c r="AJ55" s="17"/>
-      <c r="AK55" s="17"/>
-      <c r="AL55" s="26"/>
-      <c r="AM55" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN55" s="27"/>
-    </row>
-    <row r="56" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="18"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="18"/>
-      <c r="U56" s="18"/>
-      <c r="V56" s="18"/>
-      <c r="W56" s="18"/>
-      <c r="X56" s="18"/>
-      <c r="Y56" s="18"/>
-      <c r="Z56" s="18"/>
-      <c r="AA56" s="18"/>
-      <c r="AB56" s="18"/>
-      <c r="AC56" s="18"/>
-      <c r="AD56" s="17"/>
-      <c r="AE56" s="17"/>
-      <c r="AF56" s="17"/>
-      <c r="AG56" s="17"/>
-      <c r="AH56" s="25"/>
-      <c r="AI56" s="17"/>
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
-      <c r="AL56" s="26"/>
-      <c r="AM56" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN56" s="27"/>
-    </row>
-    <row r="57" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="18"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="18"/>
-      <c r="T57" s="18"/>
-      <c r="U57" s="18"/>
-      <c r="V57" s="18"/>
-      <c r="W57" s="18"/>
-      <c r="X57" s="18"/>
-      <c r="Y57" s="18"/>
-      <c r="Z57" s="18"/>
-      <c r="AA57" s="18"/>
-      <c r="AB57" s="18"/>
-      <c r="AC57" s="18"/>
-      <c r="AD57" s="17"/>
-      <c r="AE57" s="17"/>
-      <c r="AF57" s="17"/>
-      <c r="AG57" s="17"/>
-      <c r="AH57" s="25"/>
-      <c r="AI57" s="17"/>
-      <c r="AJ57" s="17"/>
-      <c r="AK57" s="17"/>
-      <c r="AL57" s="26"/>
-      <c r="AM57" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN57" s="27"/>
-    </row>
-    <row r="58" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
-      <c r="Q58" s="18"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="18"/>
-      <c r="U58" s="18"/>
-      <c r="V58" s="18"/>
-      <c r="W58" s="18"/>
-      <c r="X58" s="18"/>
-      <c r="Y58" s="18"/>
-      <c r="Z58" s="18"/>
-      <c r="AA58" s="18"/>
-      <c r="AB58" s="18"/>
-      <c r="AC58" s="18"/>
-      <c r="AD58" s="17"/>
-      <c r="AE58" s="18"/>
-      <c r="AF58" s="17"/>
-      <c r="AG58" s="17"/>
-      <c r="AH58" s="25"/>
-      <c r="AI58" s="17"/>
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
-      <c r="AL58" s="26"/>
-      <c r="AM58" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN58" s="27"/>
-    </row>
-    <row r="59" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="18"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="18"/>
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
-      <c r="T59" s="18"/>
-      <c r="U59" s="18"/>
-      <c r="V59" s="18"/>
-      <c r="W59" s="18"/>
-      <c r="X59" s="18"/>
-      <c r="Y59" s="18"/>
-      <c r="Z59" s="18"/>
-      <c r="AA59" s="18"/>
-      <c r="AB59" s="18"/>
-      <c r="AC59" s="18"/>
-      <c r="AD59" s="17"/>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
-      <c r="AG59" s="17"/>
-      <c r="AH59" s="25"/>
-      <c r="AI59" s="17"/>
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
-      <c r="AL59" s="26"/>
-      <c r="AM59" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN59" s="27"/>
-    </row>
-    <row r="60" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="18"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="17"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="18"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
-      <c r="T60" s="18"/>
-      <c r="U60" s="18"/>
-      <c r="V60" s="18"/>
-      <c r="W60" s="18"/>
-      <c r="X60" s="18"/>
-      <c r="Y60" s="18"/>
-      <c r="Z60" s="18"/>
-      <c r="AA60" s="18"/>
-      <c r="AB60" s="18"/>
-      <c r="AC60" s="18"/>
-      <c r="AD60" s="17"/>
-      <c r="AE60" s="17"/>
-      <c r="AF60" s="17"/>
-      <c r="AG60" s="17"/>
-      <c r="AH60" s="25"/>
-      <c r="AI60" s="17"/>
-      <c r="AJ60" s="17"/>
-      <c r="AK60" s="17"/>
-      <c r="AL60" s="26"/>
-      <c r="AM60" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN60" s="27"/>
-    </row>
-    <row r="61" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="18"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="24"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
-      <c r="T61" s="18"/>
-      <c r="U61" s="18"/>
-      <c r="V61" s="18"/>
-      <c r="W61" s="18"/>
-      <c r="X61" s="18"/>
-      <c r="Y61" s="18"/>
-      <c r="Z61" s="18"/>
-      <c r="AA61" s="18"/>
-      <c r="AB61" s="18"/>
-      <c r="AC61" s="18"/>
-      <c r="AD61" s="17"/>
-      <c r="AE61" s="17"/>
-      <c r="AF61" s="17"/>
-      <c r="AG61" s="17"/>
-      <c r="AH61" s="25"/>
-      <c r="AI61" s="17"/>
-      <c r="AJ61" s="17"/>
-      <c r="AK61" s="17"/>
-      <c r="AL61" s="26"/>
-      <c r="AM61" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN61" s="27"/>
-    </row>
-    <row r="62" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="18"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="24"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="18"/>
-      <c r="S62" s="18"/>
-      <c r="T62" s="18"/>
-      <c r="U62" s="18"/>
-      <c r="V62" s="18"/>
-      <c r="W62" s="18"/>
-      <c r="X62" s="18"/>
-      <c r="Y62" s="18"/>
-      <c r="Z62" s="18"/>
-      <c r="AA62" s="18"/>
-      <c r="AB62" s="18"/>
-      <c r="AC62" s="18"/>
-      <c r="AD62" s="17"/>
-      <c r="AE62" s="17"/>
-      <c r="AF62" s="17"/>
-      <c r="AG62" s="17"/>
-      <c r="AH62" s="25"/>
-      <c r="AI62" s="17"/>
-      <c r="AJ62" s="17"/>
-      <c r="AK62" s="17"/>
-      <c r="AL62" s="26"/>
-      <c r="AM62" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN62" s="27"/>
-    </row>
-    <row r="63" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="18"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="24"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="18"/>
-      <c r="T63" s="18"/>
-      <c r="U63" s="18"/>
-      <c r="V63" s="18"/>
-      <c r="W63" s="18"/>
-      <c r="X63" s="18"/>
-      <c r="Y63" s="18"/>
-      <c r="Z63" s="18"/>
-      <c r="AA63" s="18"/>
-      <c r="AB63" s="18"/>
-      <c r="AC63" s="18"/>
-      <c r="AD63" s="17"/>
-      <c r="AE63" s="17"/>
-      <c r="AF63" s="17"/>
-      <c r="AG63" s="17"/>
-      <c r="AH63" s="25"/>
-      <c r="AI63" s="17"/>
-      <c r="AJ63" s="17"/>
-      <c r="AK63" s="17"/>
-      <c r="AL63" s="26"/>
-      <c r="AM63" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN63" s="27"/>
-    </row>
-    <row r="64" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="18"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="17"/>
-      <c r="L64" s="28"/>
-      <c r="M64" s="24"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="18"/>
-      <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
-      <c r="T64" s="18"/>
-      <c r="U64" s="18"/>
-      <c r="V64" s="18"/>
-      <c r="W64" s="18"/>
-      <c r="X64" s="18"/>
-      <c r="Y64" s="18"/>
-      <c r="Z64" s="18"/>
-      <c r="AA64" s="18"/>
-      <c r="AB64" s="18"/>
-      <c r="AC64" s="18"/>
-      <c r="AD64" s="17"/>
-      <c r="AE64" s="17"/>
-      <c r="AF64" s="17"/>
-      <c r="AG64" s="17"/>
-      <c r="AH64" s="25"/>
-      <c r="AI64" s="17"/>
-      <c r="AJ64" s="17"/>
-      <c r="AK64" s="17"/>
-      <c r="AL64" s="26"/>
-      <c r="AM64" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN64" s="27"/>
-    </row>
-    <row r="65" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="23"/>
-      <c r="M65" s="24"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="18"/>
-      <c r="Q65" s="18"/>
-      <c r="R65" s="18"/>
-      <c r="S65" s="18"/>
-      <c r="T65" s="18"/>
-      <c r="U65" s="18"/>
-      <c r="V65" s="18"/>
-      <c r="W65" s="18"/>
-      <c r="X65" s="18"/>
-      <c r="Y65" s="18"/>
-      <c r="Z65" s="18"/>
-      <c r="AA65" s="18"/>
-      <c r="AB65" s="18"/>
-      <c r="AC65" s="18"/>
-      <c r="AD65" s="17"/>
-      <c r="AE65" s="18"/>
-      <c r="AF65" s="17"/>
-      <c r="AG65" s="17"/>
-      <c r="AH65" s="25"/>
-      <c r="AI65" s="17"/>
-      <c r="AJ65" s="17"/>
-      <c r="AK65" s="17"/>
-      <c r="AL65" s="26"/>
-      <c r="AM65" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN65" s="27"/>
-    </row>
-    <row r="66" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="18"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="22"/>
-      <c r="K66" s="17"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="24"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="18"/>
-      <c r="Q66" s="18"/>
-      <c r="R66" s="18"/>
-      <c r="S66" s="18"/>
-      <c r="T66" s="18"/>
-      <c r="U66" s="18"/>
-      <c r="V66" s="18"/>
-      <c r="W66" s="18"/>
-      <c r="X66" s="18"/>
-      <c r="Y66" s="18"/>
-      <c r="Z66" s="18"/>
-      <c r="AA66" s="18"/>
-      <c r="AB66" s="18"/>
-      <c r="AC66" s="18"/>
-      <c r="AD66" s="17"/>
-      <c r="AE66" s="17"/>
-      <c r="AF66" s="17"/>
-      <c r="AG66" s="17"/>
-      <c r="AH66" s="25"/>
-      <c r="AI66" s="17"/>
-      <c r="AJ66" s="17"/>
-      <c r="AK66" s="17"/>
-      <c r="AL66" s="26"/>
-      <c r="AM66" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN66" s="27"/>
-    </row>
-    <row r="67" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="24"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="18"/>
-      <c r="Q67" s="18"/>
-      <c r="R67" s="18"/>
-      <c r="S67" s="18"/>
-      <c r="T67" s="18"/>
-      <c r="U67" s="18"/>
-      <c r="V67" s="18"/>
-      <c r="W67" s="18"/>
-      <c r="X67" s="18"/>
-      <c r="Y67" s="18"/>
-      <c r="Z67" s="18"/>
-      <c r="AA67" s="18"/>
-      <c r="AB67" s="18"/>
-      <c r="AC67" s="18"/>
-      <c r="AD67" s="17"/>
-      <c r="AE67" s="18"/>
-      <c r="AF67" s="17"/>
-      <c r="AG67" s="17"/>
-      <c r="AH67" s="25"/>
-      <c r="AI67" s="17"/>
-      <c r="AJ67" s="17"/>
-      <c r="AK67" s="17"/>
-      <c r="AL67" s="26"/>
-      <c r="AM67" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN67" s="27"/>
-    </row>
-    <row r="68" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="18"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="22"/>
-      <c r="K68" s="17"/>
-      <c r="L68" s="28"/>
-      <c r="M68" s="24"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="18"/>
-      <c r="Q68" s="18"/>
-      <c r="R68" s="18"/>
-      <c r="S68" s="18"/>
-      <c r="T68" s="18"/>
-      <c r="U68" s="18"/>
-      <c r="V68" s="18"/>
-      <c r="W68" s="18"/>
-      <c r="X68" s="18"/>
-      <c r="Y68" s="18"/>
-      <c r="Z68" s="18"/>
-      <c r="AA68" s="18"/>
-      <c r="AB68" s="18"/>
-      <c r="AC68" s="18"/>
-      <c r="AD68" s="17"/>
-      <c r="AE68" s="17"/>
-      <c r="AF68" s="17"/>
-      <c r="AG68" s="17"/>
-      <c r="AH68" s="25"/>
-      <c r="AI68" s="17"/>
-      <c r="AJ68" s="17"/>
-      <c r="AK68" s="17"/>
-      <c r="AL68" s="26"/>
-      <c r="AM68" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN68" s="27"/>
-    </row>
-    <row r="69" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="18"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="22"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="24"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="18"/>
-      <c r="Q69" s="18"/>
-      <c r="R69" s="18"/>
-      <c r="S69" s="18"/>
-      <c r="T69" s="18"/>
-      <c r="U69" s="18"/>
-      <c r="V69" s="18"/>
-      <c r="W69" s="18"/>
-      <c r="X69" s="18"/>
-      <c r="Y69" s="18"/>
-      <c r="Z69" s="18"/>
-      <c r="AA69" s="18"/>
-      <c r="AB69" s="18"/>
-      <c r="AC69" s="18"/>
-      <c r="AD69" s="17"/>
-      <c r="AE69" s="17"/>
-      <c r="AF69" s="17"/>
-      <c r="AG69" s="17"/>
-      <c r="AH69" s="25"/>
-      <c r="AI69" s="17"/>
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
-      <c r="AL69" s="26"/>
-      <c r="AM69" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN69" s="27"/>
-    </row>
-    <row r="70" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="22"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="23"/>
-      <c r="M70" s="24"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="18"/>
-      <c r="R70" s="18"/>
-      <c r="S70" s="18"/>
-      <c r="T70" s="18"/>
-      <c r="U70" s="18"/>
-      <c r="V70" s="18"/>
-      <c r="W70" s="18"/>
-      <c r="X70" s="18"/>
-      <c r="Y70" s="18"/>
-      <c r="Z70" s="18"/>
-      <c r="AA70" s="18"/>
-      <c r="AB70" s="18"/>
-      <c r="AC70" s="18"/>
-      <c r="AD70" s="17"/>
-      <c r="AE70" s="18"/>
-      <c r="AF70" s="17"/>
-      <c r="AG70" s="17"/>
-      <c r="AH70" s="25"/>
-      <c r="AI70" s="17"/>
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
-      <c r="AL70" s="26"/>
-      <c r="AM70" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN70" s="27"/>
-    </row>
-    <row r="71" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="22"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="24"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="18"/>
-      <c r="Q71" s="18"/>
-      <c r="R71" s="18"/>
-      <c r="S71" s="18"/>
-      <c r="T71" s="18"/>
-      <c r="U71" s="18"/>
-      <c r="V71" s="18"/>
-      <c r="W71" s="18"/>
-      <c r="X71" s="18"/>
-      <c r="Y71" s="18"/>
-      <c r="Z71" s="18"/>
-      <c r="AA71" s="18"/>
-      <c r="AB71" s="18"/>
-      <c r="AC71" s="18"/>
-      <c r="AD71" s="17"/>
-      <c r="AE71" s="18"/>
-      <c r="AF71" s="17"/>
-      <c r="AG71" s="17"/>
-      <c r="AH71" s="25"/>
-      <c r="AI71" s="17"/>
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
-      <c r="AL71" s="26"/>
-      <c r="AM71" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN71" s="27"/>
-    </row>
-    <row r="72" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="18"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="22"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="28"/>
-      <c r="M72" s="24"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="18"/>
-      <c r="Q72" s="18"/>
-      <c r="R72" s="18"/>
-      <c r="S72" s="18"/>
-      <c r="T72" s="18"/>
-      <c r="U72" s="18"/>
-      <c r="V72" s="18"/>
-      <c r="W72" s="18"/>
-      <c r="X72" s="18"/>
-      <c r="Y72" s="18"/>
-      <c r="Z72" s="18"/>
-      <c r="AA72" s="18"/>
-      <c r="AB72" s="18"/>
-      <c r="AC72" s="18"/>
-      <c r="AD72" s="17"/>
-      <c r="AE72" s="17"/>
-      <c r="AF72" s="17"/>
-      <c r="AG72" s="17"/>
-      <c r="AH72" s="25"/>
-      <c r="AI72" s="17"/>
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
-      <c r="AL72" s="26"/>
-      <c r="AM72" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN72" s="27"/>
-    </row>
-    <row r="73" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="22"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="24"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="18"/>
-      <c r="Q73" s="18"/>
-      <c r="R73" s="18"/>
-      <c r="S73" s="18"/>
-      <c r="T73" s="18"/>
-      <c r="U73" s="18"/>
-      <c r="V73" s="18"/>
-      <c r="W73" s="18"/>
-      <c r="X73" s="18"/>
-      <c r="Y73" s="18"/>
-      <c r="Z73" s="18"/>
-      <c r="AA73" s="18"/>
-      <c r="AB73" s="18"/>
-      <c r="AC73" s="18"/>
-      <c r="AD73" s="17"/>
-      <c r="AE73" s="18"/>
-      <c r="AF73" s="17"/>
-      <c r="AG73" s="17"/>
-      <c r="AH73" s="25"/>
-      <c r="AI73" s="17"/>
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
-      <c r="AL73" s="26"/>
-      <c r="AM73" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN73" s="27"/>
-    </row>
-    <row r="74" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="23"/>
-      <c r="M74" s="24"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="18"/>
-      <c r="P74" s="18"/>
-      <c r="Q74" s="18"/>
-      <c r="R74" s="18"/>
-      <c r="S74" s="18"/>
-      <c r="T74" s="18"/>
-      <c r="U74" s="18"/>
-      <c r="V74" s="18"/>
-      <c r="W74" s="18"/>
-      <c r="X74" s="18"/>
-      <c r="Y74" s="18"/>
-      <c r="Z74" s="18"/>
-      <c r="AA74" s="18"/>
-      <c r="AB74" s="18"/>
-      <c r="AC74" s="18"/>
-      <c r="AD74" s="17"/>
-      <c r="AE74" s="18"/>
-      <c r="AF74" s="17"/>
-      <c r="AG74" s="17"/>
-      <c r="AH74" s="25"/>
-      <c r="AI74" s="17"/>
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
-      <c r="AL74" s="26"/>
-      <c r="AM74" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN74" s="27"/>
-    </row>
-    <row r="75" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="22"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="23"/>
-      <c r="M75" s="24"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="18"/>
-      <c r="P75" s="18"/>
-      <c r="Q75" s="18"/>
-      <c r="R75" s="18"/>
-      <c r="S75" s="18"/>
-      <c r="T75" s="18"/>
-      <c r="U75" s="18"/>
-      <c r="V75" s="18"/>
-      <c r="W75" s="18"/>
-      <c r="X75" s="18"/>
-      <c r="Y75" s="18"/>
-      <c r="Z75" s="18"/>
-      <c r="AA75" s="18"/>
-      <c r="AB75" s="18"/>
-      <c r="AC75" s="18"/>
-      <c r="AD75" s="17"/>
-      <c r="AE75" s="18"/>
-      <c r="AF75" s="17"/>
-      <c r="AG75" s="17"/>
-      <c r="AH75" s="25"/>
-      <c r="AI75" s="17"/>
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
-      <c r="AL75" s="26"/>
-      <c r="AM75" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN75" s="27"/>
-    </row>
-    <row r="76" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="18"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="22"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="24"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="18"/>
-      <c r="Q76" s="18"/>
-      <c r="R76" s="18"/>
-      <c r="S76" s="18"/>
-      <c r="T76" s="18"/>
-      <c r="U76" s="18"/>
-      <c r="V76" s="18"/>
-      <c r="W76" s="18"/>
-      <c r="X76" s="18"/>
-      <c r="Y76" s="18"/>
-      <c r="Z76" s="18"/>
-      <c r="AA76" s="18"/>
-      <c r="AB76" s="18"/>
-      <c r="AC76" s="18"/>
-      <c r="AD76" s="17"/>
-      <c r="AE76" s="17"/>
-      <c r="AF76" s="17"/>
-      <c r="AG76" s="17"/>
-      <c r="AH76" s="25"/>
-      <c r="AI76" s="17"/>
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
-      <c r="AL76" s="26"/>
-      <c r="AM76" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN76" s="27"/>
-    </row>
-    <row r="77" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="18"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="22"/>
-      <c r="K77" s="17"/>
-      <c r="L77" s="28"/>
-      <c r="M77" s="24"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="18"/>
-      <c r="T77" s="18"/>
-      <c r="U77" s="18"/>
-      <c r="V77" s="18"/>
-      <c r="W77" s="18"/>
-      <c r="X77" s="18"/>
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="18"/>
-      <c r="AA77" s="18"/>
-      <c r="AB77" s="18"/>
-      <c r="AC77" s="18"/>
-      <c r="AD77" s="17"/>
-      <c r="AE77" s="17"/>
-      <c r="AF77" s="17"/>
-      <c r="AG77" s="17"/>
-      <c r="AH77" s="25"/>
-      <c r="AI77" s="17"/>
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
-      <c r="AL77" s="26"/>
-      <c r="AM77" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN77" s="27"/>
-    </row>
-    <row r="78" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="22"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="23"/>
-      <c r="M78" s="24"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="18"/>
-      <c r="P78" s="18"/>
-      <c r="Q78" s="18"/>
-      <c r="R78" s="18"/>
-      <c r="S78" s="18"/>
-      <c r="T78" s="18"/>
-      <c r="U78" s="18"/>
-      <c r="V78" s="18"/>
-      <c r="W78" s="18"/>
-      <c r="X78" s="18"/>
-      <c r="Y78" s="18"/>
-      <c r="Z78" s="18"/>
-      <c r="AA78" s="18"/>
-      <c r="AB78" s="18"/>
-      <c r="AC78" s="18"/>
-      <c r="AD78" s="17"/>
-      <c r="AE78" s="18"/>
-      <c r="AF78" s="17"/>
-      <c r="AG78" s="17"/>
-      <c r="AH78" s="25"/>
-      <c r="AI78" s="17"/>
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
-      <c r="AL78" s="26"/>
-      <c r="AM78" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN78" s="27"/>
-    </row>
-    <row r="79" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="22"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="23"/>
-      <c r="M79" s="24"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="18"/>
-      <c r="P79" s="18"/>
-      <c r="Q79" s="18"/>
-      <c r="R79" s="18"/>
-      <c r="S79" s="18"/>
-      <c r="T79" s="18"/>
-      <c r="U79" s="18"/>
-      <c r="V79" s="18"/>
-      <c r="W79" s="18"/>
-      <c r="X79" s="18"/>
-      <c r="Y79" s="18"/>
-      <c r="Z79" s="18"/>
-      <c r="AA79" s="18"/>
-      <c r="AB79" s="18"/>
-      <c r="AC79" s="18"/>
-      <c r="AD79" s="17"/>
-      <c r="AE79" s="18"/>
-      <c r="AF79" s="17"/>
-      <c r="AG79" s="17"/>
-      <c r="AH79" s="25"/>
-      <c r="AI79" s="17"/>
-      <c r="AJ79" s="17"/>
-      <c r="AK79" s="17"/>
-      <c r="AL79" s="26"/>
-      <c r="AM79" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN79" s="27"/>
-    </row>
-    <row r="80" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="22"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="23"/>
-      <c r="M80" s="24"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="18"/>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="18"/>
-      <c r="R80" s="18"/>
-      <c r="S80" s="18"/>
-      <c r="T80" s="18"/>
-      <c r="U80" s="18"/>
-      <c r="V80" s="18"/>
-      <c r="W80" s="18"/>
-      <c r="X80" s="18"/>
-      <c r="Y80" s="18"/>
-      <c r="Z80" s="18"/>
-      <c r="AA80" s="18"/>
-      <c r="AB80" s="18"/>
-      <c r="AC80" s="18"/>
-      <c r="AD80" s="17"/>
-      <c r="AE80" s="18"/>
-      <c r="AF80" s="17"/>
-      <c r="AG80" s="17"/>
-      <c r="AH80" s="25"/>
-      <c r="AI80" s="17"/>
-      <c r="AJ80" s="17"/>
-      <c r="AK80" s="17"/>
-      <c r="AL80" s="26"/>
-      <c r="AM80" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN80" s="27"/>
-    </row>
-    <row r="81" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="22"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="23"/>
-      <c r="M81" s="24"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="18"/>
-      <c r="P81" s="18"/>
-      <c r="Q81" s="18"/>
-      <c r="R81" s="18"/>
-      <c r="S81" s="18"/>
-      <c r="T81" s="18"/>
-      <c r="U81" s="18"/>
-      <c r="V81" s="18"/>
-      <c r="W81" s="18"/>
-      <c r="X81" s="18"/>
-      <c r="Y81" s="18"/>
-      <c r="Z81" s="18"/>
-      <c r="AA81" s="18"/>
-      <c r="AB81" s="18"/>
-      <c r="AC81" s="18"/>
-      <c r="AD81" s="17"/>
-      <c r="AE81" s="18"/>
-      <c r="AF81" s="17"/>
-      <c r="AG81" s="17"/>
-      <c r="AH81" s="25"/>
-      <c r="AI81" s="17"/>
-      <c r="AJ81" s="17"/>
-      <c r="AK81" s="17"/>
-      <c r="AL81" s="26"/>
-      <c r="AM81" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN81" s="27"/>
-    </row>
-    <row r="82" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="18"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="22"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="23"/>
-      <c r="M82" s="24"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="18"/>
-      <c r="P82" s="18"/>
-      <c r="Q82" s="18"/>
-      <c r="R82" s="18"/>
-      <c r="S82" s="18"/>
-      <c r="T82" s="18"/>
-      <c r="U82" s="18"/>
-      <c r="V82" s="18"/>
-      <c r="W82" s="18"/>
-      <c r="X82" s="18"/>
-      <c r="Y82" s="18"/>
-      <c r="Z82" s="18"/>
-      <c r="AA82" s="18"/>
-      <c r="AB82" s="18"/>
-      <c r="AC82" s="18"/>
-      <c r="AD82" s="17"/>
-      <c r="AE82" s="18"/>
-      <c r="AF82" s="17"/>
-      <c r="AG82" s="17"/>
-      <c r="AH82" s="25"/>
-      <c r="AI82" s="17"/>
-      <c r="AJ82" s="17"/>
-      <c r="AK82" s="17"/>
-      <c r="AL82" s="26"/>
-      <c r="AM82" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN82" s="27"/>
-    </row>
-    <row r="83" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="18"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="22"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="23"/>
-      <c r="M83" s="24"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="18"/>
-      <c r="P83" s="18"/>
-      <c r="Q83" s="18"/>
-      <c r="R83" s="18"/>
-      <c r="S83" s="18"/>
-      <c r="T83" s="18"/>
-      <c r="U83" s="18"/>
-      <c r="V83" s="18"/>
-      <c r="W83" s="18"/>
-      <c r="X83" s="18"/>
-      <c r="Y83" s="18"/>
-      <c r="Z83" s="18"/>
-      <c r="AA83" s="18"/>
-      <c r="AB83" s="18"/>
-      <c r="AC83" s="18"/>
-      <c r="AD83" s="17"/>
-      <c r="AE83" s="18"/>
-      <c r="AF83" s="17"/>
-      <c r="AG83" s="17"/>
-      <c r="AH83" s="25"/>
-      <c r="AI83" s="17"/>
-      <c r="AJ83" s="17"/>
-      <c r="AK83" s="17"/>
-      <c r="AL83" s="26"/>
-      <c r="AM83" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN83" s="27"/>
-    </row>
-    <row r="84" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="18"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="22"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="28"/>
-      <c r="M84" s="24"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="18"/>
-      <c r="Q84" s="18"/>
-      <c r="R84" s="18"/>
-      <c r="S84" s="18"/>
-      <c r="T84" s="18"/>
-      <c r="U84" s="18"/>
-      <c r="V84" s="18"/>
-      <c r="W84" s="18"/>
-      <c r="X84" s="18"/>
-      <c r="Y84" s="18"/>
-      <c r="Z84" s="18"/>
-      <c r="AA84" s="18"/>
-      <c r="AB84" s="18"/>
-      <c r="AC84" s="18"/>
-      <c r="AD84" s="17"/>
-      <c r="AE84" s="17"/>
-      <c r="AF84" s="17"/>
-      <c r="AG84" s="17"/>
-      <c r="AH84" s="25"/>
-      <c r="AI84" s="17"/>
-      <c r="AJ84" s="17"/>
-      <c r="AK84" s="17"/>
-      <c r="AL84" s="26"/>
-      <c r="AM84" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN84" s="27"/>
-    </row>
-    <row r="85" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="18"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="22"/>
-      <c r="K85" s="17"/>
-      <c r="L85" s="28"/>
-      <c r="M85" s="24"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="18"/>
-      <c r="Q85" s="18"/>
-      <c r="R85" s="18"/>
-      <c r="S85" s="18"/>
-      <c r="T85" s="18"/>
-      <c r="U85" s="18"/>
-      <c r="V85" s="18"/>
-      <c r="W85" s="18"/>
-      <c r="X85" s="18"/>
-      <c r="Y85" s="18"/>
-      <c r="Z85" s="18"/>
-      <c r="AA85" s="18"/>
-      <c r="AB85" s="18"/>
-      <c r="AC85" s="18"/>
-      <c r="AD85" s="17"/>
-      <c r="AE85" s="17"/>
-      <c r="AF85" s="17"/>
-      <c r="AG85" s="17"/>
-      <c r="AH85" s="25"/>
-      <c r="AI85" s="17"/>
-      <c r="AJ85" s="17"/>
-      <c r="AK85" s="17"/>
-      <c r="AL85" s="26"/>
-      <c r="AM85" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN85" s="27"/>
-    </row>
-    <row r="86" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="22"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="24"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="18"/>
-      <c r="P86" s="18"/>
-      <c r="Q86" s="18"/>
-      <c r="R86" s="18"/>
-      <c r="S86" s="18"/>
-      <c r="T86" s="18"/>
-      <c r="U86" s="18"/>
-      <c r="V86" s="18"/>
-      <c r="W86" s="18"/>
-      <c r="X86" s="18"/>
-      <c r="Y86" s="18"/>
-      <c r="Z86" s="18"/>
-      <c r="AA86" s="18"/>
-      <c r="AB86" s="18"/>
-      <c r="AC86" s="18"/>
-      <c r="AD86" s="17"/>
-      <c r="AE86" s="18"/>
-      <c r="AF86" s="17"/>
-      <c r="AG86" s="17"/>
-      <c r="AH86" s="25"/>
-      <c r="AI86" s="17"/>
-      <c r="AJ86" s="17"/>
-      <c r="AK86" s="17"/>
-      <c r="AL86" s="26"/>
-      <c r="AM86" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN86" s="27"/>
-    </row>
-    <row r="87" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="22"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="24"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="18"/>
-      <c r="P87" s="18"/>
-      <c r="Q87" s="18"/>
-      <c r="R87" s="18"/>
-      <c r="S87" s="18"/>
-      <c r="T87" s="18"/>
-      <c r="U87" s="18"/>
-      <c r="V87" s="18"/>
-      <c r="W87" s="18"/>
-      <c r="X87" s="18"/>
-      <c r="Y87" s="18"/>
-      <c r="Z87" s="18"/>
-      <c r="AA87" s="18"/>
-      <c r="AB87" s="18"/>
-      <c r="AC87" s="18"/>
-      <c r="AD87" s="17"/>
-      <c r="AE87" s="18"/>
-      <c r="AF87" s="17"/>
-      <c r="AG87" s="17"/>
-      <c r="AH87" s="25"/>
-      <c r="AI87" s="17"/>
-      <c r="AJ87" s="17"/>
-      <c r="AK87" s="17"/>
-      <c r="AL87" s="26"/>
-      <c r="AM87" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN87" s="27"/>
-    </row>
-    <row r="88" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="22"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="23"/>
-      <c r="M88" s="24"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="18"/>
-      <c r="P88" s="18"/>
-      <c r="Q88" s="18"/>
-      <c r="R88" s="18"/>
-      <c r="S88" s="18"/>
-      <c r="T88" s="18"/>
-      <c r="U88" s="18"/>
-      <c r="V88" s="18"/>
-      <c r="W88" s="18"/>
-      <c r="X88" s="18"/>
-      <c r="Y88" s="18"/>
-      <c r="Z88" s="18"/>
-      <c r="AA88" s="18"/>
-      <c r="AB88" s="18"/>
-      <c r="AC88" s="18"/>
-      <c r="AD88" s="17"/>
-      <c r="AE88" s="18"/>
-      <c r="AF88" s="17"/>
-      <c r="AG88" s="17"/>
-      <c r="AH88" s="25"/>
-      <c r="AI88" s="17"/>
-      <c r="AJ88" s="17"/>
-      <c r="AK88" s="17"/>
-      <c r="AL88" s="26"/>
-      <c r="AM88" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN88" s="27"/>
-    </row>
-    <row r="89" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="22"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="24"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-      <c r="R89" s="18"/>
-      <c r="S89" s="18"/>
-      <c r="T89" s="18"/>
-      <c r="U89" s="18"/>
-      <c r="V89" s="18"/>
-      <c r="W89" s="18"/>
-      <c r="X89" s="18"/>
-      <c r="Y89" s="18"/>
-      <c r="Z89" s="18"/>
-      <c r="AA89" s="18"/>
-      <c r="AB89" s="18"/>
-      <c r="AC89" s="18"/>
-      <c r="AD89" s="17"/>
-      <c r="AE89" s="18"/>
-      <c r="AF89" s="17"/>
-      <c r="AG89" s="17"/>
-      <c r="AH89" s="25"/>
-      <c r="AI89" s="17"/>
-      <c r="AJ89" s="17"/>
-      <c r="AK89" s="17"/>
-      <c r="AL89" s="26"/>
-      <c r="AM89" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN89" s="27"/>
-    </row>
-    <row r="90" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="18"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="22"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="24"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="18"/>
-      <c r="Q90" s="18"/>
-      <c r="R90" s="18"/>
-      <c r="S90" s="18"/>
-      <c r="T90" s="18"/>
-      <c r="U90" s="18"/>
-      <c r="V90" s="18"/>
-      <c r="W90" s="18"/>
-      <c r="X90" s="18"/>
-      <c r="Y90" s="18"/>
-      <c r="Z90" s="18"/>
-      <c r="AA90" s="18"/>
-      <c r="AB90" s="18"/>
-      <c r="AC90" s="18"/>
-      <c r="AD90" s="17"/>
-      <c r="AE90" s="17"/>
-      <c r="AF90" s="17"/>
-      <c r="AG90" s="17"/>
-      <c r="AH90" s="25"/>
-      <c r="AI90" s="17"/>
-      <c r="AJ90" s="17"/>
-      <c r="AK90" s="17"/>
-      <c r="AL90" s="26"/>
-      <c r="AM90" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN90" s="27"/>
-    </row>
-    <row r="91" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="18"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="22"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="18"/>
-      <c r="Q91" s="18"/>
-      <c r="R91" s="18"/>
-      <c r="S91" s="18"/>
-      <c r="T91" s="18"/>
-      <c r="U91" s="18"/>
-      <c r="V91" s="18"/>
-      <c r="W91" s="18"/>
-      <c r="X91" s="18"/>
-      <c r="Y91" s="18"/>
-      <c r="Z91" s="18"/>
-      <c r="AA91" s="18"/>
-      <c r="AB91" s="18"/>
-      <c r="AC91" s="18"/>
-      <c r="AD91" s="17"/>
-      <c r="AE91" s="17"/>
-      <c r="AF91" s="17"/>
-      <c r="AG91" s="17"/>
-      <c r="AH91" s="25"/>
-      <c r="AI91" s="17"/>
-      <c r="AJ91" s="17"/>
-      <c r="AK91" s="17"/>
-      <c r="AL91" s="26"/>
-      <c r="AM91" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN91" s="27"/>
-    </row>
-    <row r="92" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="18"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="17"/>
-      <c r="J92" s="22"/>
-      <c r="K92" s="17"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="24"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="18"/>
-      <c r="Q92" s="18"/>
-      <c r="R92" s="18"/>
-      <c r="S92" s="18"/>
-      <c r="T92" s="18"/>
-      <c r="U92" s="18"/>
-      <c r="V92" s="18"/>
-      <c r="W92" s="18"/>
-      <c r="X92" s="18"/>
-      <c r="Y92" s="18"/>
-      <c r="Z92" s="18"/>
-      <c r="AA92" s="18"/>
-      <c r="AB92" s="18"/>
-      <c r="AC92" s="18"/>
-      <c r="AD92" s="17"/>
-      <c r="AE92" s="17"/>
-      <c r="AF92" s="17"/>
-      <c r="AG92" s="17"/>
-      <c r="AH92" s="25"/>
-      <c r="AI92" s="17"/>
-      <c r="AJ92" s="17"/>
-      <c r="AK92" s="17"/>
-      <c r="AL92" s="26"/>
-      <c r="AM92" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN92" s="27"/>
-    </row>
-    <row r="93" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="18"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="22"/>
-      <c r="K93" s="17"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="24"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="18"/>
-      <c r="Q93" s="18"/>
-      <c r="R93" s="18"/>
-      <c r="S93" s="18"/>
-      <c r="T93" s="18"/>
-      <c r="U93" s="18"/>
-      <c r="V93" s="18"/>
-      <c r="W93" s="18"/>
-      <c r="X93" s="18"/>
-      <c r="Y93" s="18"/>
-      <c r="Z93" s="18"/>
-      <c r="AA93" s="18"/>
-      <c r="AB93" s="18"/>
-      <c r="AC93" s="18"/>
-      <c r="AD93" s="17"/>
-      <c r="AE93" s="17"/>
-      <c r="AF93" s="17"/>
-      <c r="AG93" s="17"/>
-      <c r="AH93" s="25"/>
-      <c r="AI93" s="17"/>
-      <c r="AJ93" s="17"/>
-      <c r="AK93" s="17"/>
-      <c r="AL93" s="26"/>
-      <c r="AM93" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN93" s="27"/>
-    </row>
-    <row r="94" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="18"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="17"/>
-      <c r="J94" s="22"/>
-      <c r="K94" s="17"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="24"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="18"/>
-      <c r="Q94" s="18"/>
-      <c r="R94" s="18"/>
-      <c r="S94" s="18"/>
-      <c r="T94" s="18"/>
-      <c r="U94" s="18"/>
-      <c r="V94" s="18"/>
-      <c r="W94" s="18"/>
-      <c r="X94" s="18"/>
-      <c r="Y94" s="18"/>
-      <c r="Z94" s="18"/>
-      <c r="AA94" s="18"/>
-      <c r="AB94" s="18"/>
-      <c r="AC94" s="18"/>
-      <c r="AD94" s="17"/>
-      <c r="AE94" s="17"/>
-      <c r="AF94" s="17"/>
-      <c r="AG94" s="17"/>
-      <c r="AH94" s="25"/>
-      <c r="AI94" s="17"/>
-      <c r="AJ94" s="17"/>
-      <c r="AK94" s="17"/>
-      <c r="AL94" s="26"/>
-      <c r="AM94" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN94" s="27"/>
-    </row>
-    <row r="95" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="18"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="22"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="24"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="18"/>
-      <c r="Q95" s="18"/>
-      <c r="R95" s="18"/>
-      <c r="S95" s="18"/>
-      <c r="T95" s="18"/>
-      <c r="U95" s="18"/>
-      <c r="V95" s="18"/>
-      <c r="W95" s="18"/>
-      <c r="X95" s="18"/>
-      <c r="Y95" s="18"/>
-      <c r="Z95" s="18"/>
-      <c r="AA95" s="18"/>
-      <c r="AB95" s="18"/>
-      <c r="AC95" s="18"/>
-      <c r="AD95" s="17"/>
-      <c r="AE95" s="17"/>
-      <c r="AF95" s="17"/>
-      <c r="AG95" s="17"/>
-      <c r="AH95" s="25"/>
-      <c r="AI95" s="17"/>
-      <c r="AJ95" s="17"/>
-      <c r="AK95" s="17"/>
-      <c r="AL95" s="26"/>
-      <c r="AM95" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN95" s="27"/>
-    </row>
-    <row r="96" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="18"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="18"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="22"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="24"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="18"/>
-      <c r="Q96" s="18"/>
-      <c r="R96" s="18"/>
-      <c r="S96" s="18"/>
-      <c r="T96" s="18"/>
-      <c r="U96" s="18"/>
-      <c r="V96" s="18"/>
-      <c r="W96" s="18"/>
-      <c r="X96" s="18"/>
-      <c r="Y96" s="18"/>
-      <c r="Z96" s="18"/>
-      <c r="AA96" s="18"/>
-      <c r="AB96" s="18"/>
-      <c r="AC96" s="18"/>
-      <c r="AD96" s="17"/>
-      <c r="AE96" s="17"/>
-      <c r="AF96" s="17"/>
-      <c r="AG96" s="17"/>
-      <c r="AH96" s="25"/>
-      <c r="AI96" s="17"/>
-      <c r="AJ96" s="17"/>
-      <c r="AK96" s="17"/>
-      <c r="AL96" s="26"/>
-      <c r="AM96" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN96" s="27"/>
-    </row>
-    <row r="97" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="18"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="22"/>
-      <c r="K97" s="17"/>
-      <c r="L97" s="28"/>
-      <c r="M97" s="24"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="18"/>
-      <c r="Q97" s="18"/>
-      <c r="R97" s="18"/>
-      <c r="S97" s="18"/>
-      <c r="T97" s="18"/>
-      <c r="U97" s="18"/>
-      <c r="V97" s="18"/>
-      <c r="W97" s="18"/>
-      <c r="X97" s="18"/>
-      <c r="Y97" s="18"/>
-      <c r="Z97" s="18"/>
-      <c r="AA97" s="18"/>
-      <c r="AB97" s="18"/>
-      <c r="AC97" s="18"/>
-      <c r="AD97" s="17"/>
-      <c r="AE97" s="17"/>
-      <c r="AF97" s="17"/>
-      <c r="AG97" s="17"/>
-      <c r="AH97" s="25"/>
-      <c r="AI97" s="17"/>
-      <c r="AJ97" s="17"/>
-      <c r="AK97" s="17"/>
-      <c r="AL97" s="26"/>
-      <c r="AM97" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN97" s="27"/>
-    </row>
-    <row r="98" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="22"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="23"/>
-      <c r="M98" s="24"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="18"/>
-      <c r="P98" s="18"/>
-      <c r="Q98" s="18"/>
-      <c r="R98" s="18"/>
-      <c r="S98" s="18"/>
-      <c r="T98" s="18"/>
-      <c r="U98" s="18"/>
-      <c r="V98" s="18"/>
-      <c r="W98" s="18"/>
-      <c r="X98" s="18"/>
-      <c r="Y98" s="18"/>
-      <c r="Z98" s="18"/>
-      <c r="AA98" s="18"/>
-      <c r="AB98" s="18"/>
-      <c r="AC98" s="18"/>
-      <c r="AD98" s="17"/>
-      <c r="AE98" s="18"/>
-      <c r="AF98" s="17"/>
-      <c r="AG98" s="17"/>
-      <c r="AH98" s="25"/>
-      <c r="AI98" s="17"/>
-      <c r="AJ98" s="17"/>
-      <c r="AK98" s="17"/>
-      <c r="AL98" s="26"/>
-      <c r="AM98" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN98" s="27"/>
-    </row>
-    <row r="99" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="18"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="21"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="18"/>
-      <c r="I99" s="17"/>
-      <c r="J99" s="22"/>
-      <c r="K99" s="17"/>
-      <c r="L99" s="28"/>
-      <c r="M99" s="24"/>
-      <c r="N99" s="17"/>
-      <c r="O99" s="17"/>
-      <c r="P99" s="18"/>
-      <c r="Q99" s="18"/>
-      <c r="R99" s="18"/>
-      <c r="S99" s="18"/>
-      <c r="T99" s="18"/>
-      <c r="U99" s="18"/>
-      <c r="V99" s="18"/>
-      <c r="W99" s="18"/>
-      <c r="X99" s="18"/>
-      <c r="Y99" s="18"/>
-      <c r="Z99" s="18"/>
-      <c r="AA99" s="18"/>
-      <c r="AB99" s="18"/>
-      <c r="AC99" s="18"/>
-      <c r="AD99" s="17"/>
-      <c r="AE99" s="17"/>
-      <c r="AF99" s="17"/>
-      <c r="AG99" s="17"/>
-      <c r="AH99" s="25"/>
-      <c r="AI99" s="17"/>
-      <c r="AJ99" s="17"/>
-      <c r="AK99" s="17"/>
-      <c r="AL99" s="26"/>
-      <c r="AM99" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN99" s="27"/>
-    </row>
-    <row r="100" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="21"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="17"/>
-      <c r="J100" s="22"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="23"/>
-      <c r="M100" s="24"/>
-      <c r="N100" s="17"/>
-      <c r="O100" s="18"/>
-      <c r="P100" s="18"/>
-      <c r="Q100" s="18"/>
-      <c r="R100" s="18"/>
-      <c r="S100" s="18"/>
-      <c r="T100" s="18"/>
-      <c r="U100" s="18"/>
-      <c r="V100" s="18"/>
-      <c r="W100" s="18"/>
-      <c r="X100" s="18"/>
-      <c r="Y100" s="18"/>
-      <c r="Z100" s="18"/>
-      <c r="AA100" s="18"/>
-      <c r="AB100" s="18"/>
-      <c r="AC100" s="18"/>
-      <c r="AD100" s="17"/>
-      <c r="AE100" s="18"/>
-      <c r="AF100" s="17"/>
-      <c r="AG100" s="17"/>
-      <c r="AH100" s="25"/>
-      <c r="AI100" s="17"/>
-      <c r="AJ100" s="17"/>
-      <c r="AK100" s="17"/>
-      <c r="AL100" s="26"/>
-      <c r="AM100" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN100" s="27"/>
-    </row>
-    <row r="101" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="18"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="21"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="17"/>
-      <c r="J101" s="22"/>
-      <c r="K101" s="17"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="24"/>
-      <c r="N101" s="17"/>
-      <c r="O101" s="17"/>
-      <c r="P101" s="18"/>
-      <c r="Q101" s="18"/>
-      <c r="R101" s="18"/>
-      <c r="S101" s="18"/>
-      <c r="T101" s="18"/>
-      <c r="U101" s="18"/>
-      <c r="V101" s="18"/>
-      <c r="W101" s="18"/>
-      <c r="X101" s="18"/>
-      <c r="Y101" s="18"/>
-      <c r="Z101" s="18"/>
-      <c r="AA101" s="18"/>
-      <c r="AB101" s="18"/>
-      <c r="AC101" s="18"/>
-      <c r="AD101" s="17"/>
-      <c r="AE101" s="17"/>
-      <c r="AF101" s="17"/>
-      <c r="AG101" s="17"/>
-      <c r="AH101" s="25"/>
-      <c r="AI101" s="17"/>
-      <c r="AJ101" s="17"/>
-      <c r="AK101" s="17"/>
-      <c r="AL101" s="26"/>
-      <c r="AM101" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN101" s="27"/>
-    </row>
-    <row r="102" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="18"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="21"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="17"/>
-      <c r="J102" s="22"/>
-      <c r="K102" s="17"/>
-      <c r="L102" s="28"/>
-      <c r="M102" s="24"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
-      <c r="P102" s="18"/>
-      <c r="Q102" s="18"/>
-      <c r="R102" s="18"/>
-      <c r="S102" s="18"/>
-      <c r="T102" s="18"/>
-      <c r="U102" s="18"/>
-      <c r="V102" s="18"/>
-      <c r="W102" s="18"/>
-      <c r="X102" s="18"/>
-      <c r="Y102" s="18"/>
-      <c r="Z102" s="18"/>
-      <c r="AA102" s="18"/>
-      <c r="AB102" s="18"/>
-      <c r="AC102" s="18"/>
-      <c r="AD102" s="17"/>
-      <c r="AE102" s="17"/>
-      <c r="AF102" s="17"/>
-      <c r="AG102" s="17"/>
-      <c r="AH102" s="25"/>
-      <c r="AI102" s="17"/>
-      <c r="AJ102" s="17"/>
-      <c r="AK102" s="17"/>
-      <c r="AL102" s="26"/>
-      <c r="AM102" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN102" s="27"/>
-    </row>
-    <row r="103" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="18"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="17"/>
-      <c r="J103" s="22"/>
-      <c r="K103" s="17"/>
-      <c r="L103" s="28"/>
-      <c r="M103" s="24"/>
-      <c r="N103" s="17"/>
-      <c r="O103" s="17"/>
-      <c r="P103" s="18"/>
-      <c r="Q103" s="18"/>
-      <c r="R103" s="18"/>
-      <c r="S103" s="18"/>
-      <c r="T103" s="18"/>
-      <c r="U103" s="18"/>
-      <c r="V103" s="18"/>
-      <c r="W103" s="18"/>
-      <c r="X103" s="18"/>
-      <c r="Y103" s="18"/>
-      <c r="Z103" s="18"/>
-      <c r="AA103" s="18"/>
-      <c r="AB103" s="18"/>
-      <c r="AC103" s="18"/>
-      <c r="AD103" s="17"/>
-      <c r="AE103" s="17"/>
-      <c r="AF103" s="17"/>
-      <c r="AG103" s="17"/>
-      <c r="AH103" s="25"/>
-      <c r="AI103" s="17"/>
-      <c r="AJ103" s="17"/>
-      <c r="AK103" s="17"/>
-      <c r="AL103" s="26"/>
-      <c r="AM103" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN103" s="27"/>
-    </row>
-    <row r="104" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="18"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="21"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="18"/>
-      <c r="I104" s="17"/>
-      <c r="J104" s="22"/>
-      <c r="K104" s="17"/>
-      <c r="L104" s="28"/>
-      <c r="M104" s="24"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="18"/>
-      <c r="Q104" s="18"/>
-      <c r="R104" s="18"/>
-      <c r="S104" s="18"/>
-      <c r="T104" s="18"/>
-      <c r="U104" s="18"/>
-      <c r="V104" s="18"/>
-      <c r="W104" s="18"/>
-      <c r="X104" s="18"/>
-      <c r="Y104" s="18"/>
-      <c r="Z104" s="18"/>
-      <c r="AA104" s="18"/>
-      <c r="AB104" s="18"/>
-      <c r="AC104" s="18"/>
-      <c r="AD104" s="17"/>
-      <c r="AE104" s="17"/>
-      <c r="AF104" s="17"/>
-      <c r="AG104" s="17"/>
-      <c r="AH104" s="25"/>
-      <c r="AI104" s="17"/>
-      <c r="AJ104" s="17"/>
-      <c r="AK104" s="17"/>
-      <c r="AL104" s="26"/>
-      <c r="AM104" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN104" s="27"/>
-    </row>
-    <row r="105" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="18"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="17"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="17"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="17"/>
-      <c r="J105" s="22"/>
-      <c r="K105" s="17"/>
-      <c r="L105" s="28"/>
-      <c r="M105" s="24"/>
-      <c r="N105" s="17"/>
-      <c r="O105" s="17"/>
-      <c r="P105" s="18"/>
-      <c r="Q105" s="18"/>
-      <c r="R105" s="18"/>
-      <c r="S105" s="18"/>
-      <c r="T105" s="18"/>
-      <c r="U105" s="18"/>
-      <c r="V105" s="18"/>
-      <c r="W105" s="18"/>
-      <c r="X105" s="18"/>
-      <c r="Y105" s="18"/>
-      <c r="Z105" s="18"/>
-      <c r="AA105" s="18"/>
-      <c r="AB105" s="18"/>
-      <c r="AC105" s="18"/>
-      <c r="AD105" s="17"/>
-      <c r="AE105" s="17"/>
-      <c r="AF105" s="17"/>
-      <c r="AG105" s="17"/>
-      <c r="AH105" s="25"/>
-      <c r="AI105" s="17"/>
-      <c r="AJ105" s="17"/>
-      <c r="AK105" s="17"/>
-      <c r="AL105" s="26"/>
-      <c r="AM105" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN105" s="27"/>
-    </row>
-    <row r="106" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="18"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="17"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="17"/>
-      <c r="J106" s="22"/>
-      <c r="K106" s="17"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="24"/>
-      <c r="N106" s="17"/>
-      <c r="O106" s="17"/>
-      <c r="P106" s="18"/>
-      <c r="Q106" s="18"/>
-      <c r="R106" s="18"/>
-      <c r="S106" s="18"/>
-      <c r="T106" s="18"/>
-      <c r="U106" s="18"/>
-      <c r="V106" s="18"/>
-      <c r="W106" s="18"/>
-      <c r="X106" s="18"/>
-      <c r="Y106" s="18"/>
-      <c r="Z106" s="18"/>
-      <c r="AA106" s="18"/>
-      <c r="AB106" s="18"/>
-      <c r="AC106" s="18"/>
-      <c r="AD106" s="17"/>
-      <c r="AE106" s="17"/>
-      <c r="AF106" s="17"/>
-      <c r="AG106" s="17"/>
-      <c r="AH106" s="25"/>
-      <c r="AI106" s="17"/>
-      <c r="AJ106" s="17"/>
-      <c r="AK106" s="17"/>
-      <c r="AL106" s="26"/>
-      <c r="AM106" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN106" s="27"/>
-    </row>
-    <row r="107" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="18"/>
-      <c r="H107" s="18"/>
-      <c r="I107" s="17"/>
-      <c r="J107" s="22"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="23"/>
-      <c r="M107" s="24"/>
-      <c r="N107" s="17"/>
-      <c r="O107" s="18"/>
-      <c r="P107" s="18"/>
-      <c r="Q107" s="18"/>
-      <c r="R107" s="18"/>
-      <c r="S107" s="18"/>
-      <c r="T107" s="18"/>
-      <c r="U107" s="18"/>
-      <c r="V107" s="18"/>
-      <c r="W107" s="18"/>
-      <c r="X107" s="18"/>
-      <c r="Y107" s="18"/>
-      <c r="Z107" s="18"/>
-      <c r="AA107" s="18"/>
-      <c r="AB107" s="18"/>
-      <c r="AC107" s="18"/>
-      <c r="AD107" s="17"/>
-      <c r="AE107" s="18"/>
-      <c r="AF107" s="17"/>
-      <c r="AG107" s="17"/>
-      <c r="AH107" s="25"/>
-      <c r="AI107" s="17"/>
-      <c r="AJ107" s="17"/>
-      <c r="AK107" s="17"/>
-      <c r="AL107" s="26"/>
-      <c r="AM107" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN107" s="27"/>
-    </row>
-    <row r="108" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="17"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="18"/>
-      <c r="H108" s="18"/>
-      <c r="I108" s="17"/>
-      <c r="J108" s="22"/>
-      <c r="K108" s="23"/>
-      <c r="L108" s="23"/>
-      <c r="M108" s="24"/>
-      <c r="N108" s="17"/>
-      <c r="O108" s="18"/>
-      <c r="P108" s="18"/>
-      <c r="Q108" s="18"/>
-      <c r="R108" s="18"/>
-      <c r="S108" s="18"/>
-      <c r="T108" s="18"/>
-      <c r="U108" s="18"/>
-      <c r="V108" s="18"/>
-      <c r="W108" s="18"/>
-      <c r="X108" s="18"/>
-      <c r="Y108" s="18"/>
-      <c r="Z108" s="18"/>
-      <c r="AA108" s="18"/>
-      <c r="AB108" s="18"/>
-      <c r="AC108" s="18"/>
-      <c r="AD108" s="17"/>
-      <c r="AE108" s="18"/>
-      <c r="AF108" s="17"/>
-      <c r="AG108" s="17"/>
-      <c r="AH108" s="25"/>
-      <c r="AI108" s="17"/>
-      <c r="AJ108" s="17"/>
-      <c r="AK108" s="17"/>
-      <c r="AL108" s="26"/>
-      <c r="AM108" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN108" s="27"/>
-    </row>
-    <row r="109" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="21"/>
-      <c r="G109" s="18"/>
-      <c r="H109" s="18"/>
-      <c r="I109" s="17"/>
-      <c r="J109" s="22"/>
-      <c r="K109" s="23"/>
-      <c r="L109" s="23"/>
-      <c r="M109" s="24"/>
-      <c r="N109" s="17"/>
-      <c r="O109" s="18"/>
-      <c r="P109" s="18"/>
-      <c r="Q109" s="18"/>
-      <c r="R109" s="18"/>
-      <c r="S109" s="18"/>
-      <c r="T109" s="18"/>
-      <c r="U109" s="18"/>
-      <c r="V109" s="18"/>
-      <c r="W109" s="18"/>
-      <c r="X109" s="18"/>
-      <c r="Y109" s="18"/>
-      <c r="Z109" s="18"/>
-      <c r="AA109" s="18"/>
-      <c r="AB109" s="18"/>
-      <c r="AC109" s="18"/>
-      <c r="AD109" s="17"/>
-      <c r="AE109" s="18"/>
-      <c r="AF109" s="17"/>
-      <c r="AG109" s="17"/>
-      <c r="AH109" s="25"/>
-      <c r="AI109" s="17"/>
-      <c r="AJ109" s="17"/>
-      <c r="AK109" s="17"/>
-      <c r="AL109" s="26"/>
-      <c r="AM109" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN109" s="27"/>
-    </row>
-    <row r="110" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="18"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="17"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="21"/>
-      <c r="G110" s="17"/>
-      <c r="H110" s="18"/>
-      <c r="I110" s="17"/>
-      <c r="J110" s="22"/>
-      <c r="K110" s="17"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="24"/>
-      <c r="N110" s="17"/>
-      <c r="O110" s="17"/>
-      <c r="P110" s="18"/>
-      <c r="Q110" s="18"/>
-      <c r="R110" s="18"/>
-      <c r="S110" s="18"/>
-      <c r="T110" s="18"/>
-      <c r="U110" s="18"/>
-      <c r="V110" s="18"/>
-      <c r="W110" s="18"/>
-      <c r="X110" s="18"/>
-      <c r="Y110" s="18"/>
-      <c r="Z110" s="18"/>
-      <c r="AA110" s="18"/>
-      <c r="AB110" s="18"/>
-      <c r="AC110" s="18"/>
-      <c r="AD110" s="17"/>
-      <c r="AE110" s="17"/>
-      <c r="AF110" s="17"/>
-      <c r="AG110" s="17"/>
-      <c r="AH110" s="25"/>
-      <c r="AI110" s="17"/>
-      <c r="AJ110" s="17"/>
-      <c r="AK110" s="17"/>
-      <c r="AL110" s="26"/>
-      <c r="AM110" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN110" s="27"/>
-    </row>
-    <row r="111" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="21"/>
-      <c r="G111" s="18"/>
-      <c r="H111" s="18"/>
-      <c r="I111" s="17"/>
-      <c r="J111" s="22"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="23"/>
-      <c r="M111" s="24"/>
-      <c r="N111" s="17"/>
-      <c r="O111" s="18"/>
-      <c r="P111" s="18"/>
-      <c r="Q111" s="18"/>
-      <c r="R111" s="18"/>
-      <c r="S111" s="18"/>
-      <c r="T111" s="18"/>
-      <c r="U111" s="18"/>
-      <c r="V111" s="18"/>
-      <c r="W111" s="18"/>
-      <c r="X111" s="18"/>
-      <c r="Y111" s="18"/>
-      <c r="Z111" s="18"/>
-      <c r="AA111" s="18"/>
-      <c r="AB111" s="18"/>
-      <c r="AC111" s="18"/>
-      <c r="AD111" s="17"/>
-      <c r="AE111" s="18"/>
-      <c r="AF111" s="17"/>
-      <c r="AG111" s="17"/>
-      <c r="AH111" s="25"/>
-      <c r="AI111" s="17"/>
-      <c r="AJ111" s="17"/>
-      <c r="AK111" s="17"/>
-      <c r="AL111" s="26"/>
-      <c r="AM111" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN111" s="27"/>
-    </row>
-    <row r="112" spans="2:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="18"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="21"/>
-      <c r="G112" s="18"/>
-      <c r="H112" s="18"/>
-      <c r="I112" s="17"/>
-      <c r="J112" s="22"/>
-      <c r="K112" s="23"/>
-      <c r="L112" s="23"/>
-      <c r="M112" s="24"/>
-      <c r="N112" s="17"/>
-      <c r="O112" s="18"/>
-      <c r="P112" s="18"/>
-      <c r="Q112" s="18"/>
-      <c r="R112" s="18"/>
-      <c r="S112" s="18"/>
-      <c r="T112" s="18"/>
-      <c r="U112" s="18"/>
-      <c r="V112" s="18"/>
-      <c r="W112" s="18"/>
-      <c r="X112" s="18"/>
-      <c r="Y112" s="18"/>
-      <c r="Z112" s="18"/>
-      <c r="AA112" s="18"/>
-      <c r="AB112" s="18"/>
-      <c r="AC112" s="18"/>
-      <c r="AD112" s="17"/>
-      <c r="AE112" s="18"/>
-      <c r="AF112" s="17"/>
-      <c r="AG112" s="17"/>
-      <c r="AH112" s="25"/>
-      <c r="AI112" s="17"/>
-      <c r="AJ112" s="17"/>
-      <c r="AK112" s="17"/>
-      <c r="AL112" s="26"/>
-      <c r="AM112" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN112" s="27"/>
-    </row>
-    <row r="113" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="18"/>
-      <c r="C113" s="17"/>
-      <c r="D113" s="17"/>
-      <c r="E113" s="17"/>
-      <c r="F113" s="21"/>
-      <c r="G113" s="17"/>
-      <c r="H113" s="18"/>
-      <c r="I113" s="17"/>
-      <c r="J113" s="22"/>
-      <c r="K113" s="17"/>
-      <c r="L113" s="28"/>
-      <c r="M113" s="24"/>
-      <c r="N113" s="17"/>
-      <c r="O113" s="17"/>
-      <c r="P113" s="18"/>
-      <c r="Q113" s="18"/>
-      <c r="R113" s="18"/>
-      <c r="S113" s="18"/>
-      <c r="T113" s="18"/>
-      <c r="U113" s="18"/>
-      <c r="V113" s="18"/>
-      <c r="W113" s="18"/>
-      <c r="X113" s="18"/>
-      <c r="Y113" s="18"/>
-      <c r="Z113" s="18"/>
-      <c r="AA113" s="18"/>
-      <c r="AB113" s="18"/>
-      <c r="AC113" s="18"/>
-      <c r="AD113" s="17"/>
-      <c r="AE113" s="17"/>
-      <c r="AF113" s="17"/>
-      <c r="AG113" s="17"/>
-      <c r="AH113" s="25"/>
-      <c r="AI113" s="17"/>
-      <c r="AJ113" s="17"/>
-      <c r="AK113" s="17"/>
-      <c r="AL113" s="26"/>
-      <c r="AM113" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN113" s="27"/>
-    </row>
-    <row r="114" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="18"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="21"/>
-      <c r="G114" s="17"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="17"/>
-      <c r="J114" s="22"/>
-      <c r="K114" s="17"/>
-      <c r="L114" s="28"/>
-      <c r="M114" s="24"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="17"/>
-      <c r="P114" s="18"/>
-      <c r="Q114" s="18"/>
-      <c r="R114" s="18"/>
-      <c r="S114" s="18"/>
-      <c r="T114" s="18"/>
-      <c r="U114" s="18"/>
-      <c r="V114" s="18"/>
-      <c r="W114" s="18"/>
-      <c r="X114" s="18"/>
-      <c r="Y114" s="18"/>
-      <c r="Z114" s="18"/>
-      <c r="AA114" s="18"/>
-      <c r="AB114" s="18"/>
-      <c r="AC114" s="18"/>
-      <c r="AD114" s="17"/>
-      <c r="AE114" s="17"/>
-      <c r="AF114" s="17"/>
-      <c r="AG114" s="17"/>
-      <c r="AH114" s="25"/>
-      <c r="AI114" s="17"/>
-      <c r="AJ114" s="17"/>
-      <c r="AK114" s="17"/>
-      <c r="AL114" s="26"/>
-      <c r="AM114" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN114" s="27"/>
-    </row>
-    <row r="115" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="18"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="21"/>
-      <c r="G115" s="17"/>
-      <c r="H115" s="18"/>
-      <c r="I115" s="17"/>
-      <c r="J115" s="22"/>
-      <c r="K115" s="17"/>
-      <c r="L115" s="28"/>
-      <c r="M115" s="24"/>
-      <c r="N115" s="17"/>
-      <c r="O115" s="17"/>
-      <c r="P115" s="18"/>
-      <c r="Q115" s="18"/>
-      <c r="R115" s="18"/>
-      <c r="S115" s="18"/>
-      <c r="T115" s="18"/>
-      <c r="U115" s="18"/>
-      <c r="V115" s="18"/>
-      <c r="W115" s="18"/>
-      <c r="X115" s="18"/>
-      <c r="Y115" s="18"/>
-      <c r="Z115" s="18"/>
-      <c r="AA115" s="18"/>
-      <c r="AB115" s="18"/>
-      <c r="AC115" s="18"/>
-      <c r="AD115" s="17"/>
-      <c r="AE115" s="17"/>
-      <c r="AF115" s="17"/>
-      <c r="AG115" s="17"/>
-      <c r="AH115" s="25"/>
-      <c r="AI115" s="17"/>
-      <c r="AJ115" s="17"/>
-      <c r="AK115" s="17"/>
-      <c r="AL115" s="26"/>
-      <c r="AM115" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN115" s="27"/>
-    </row>
-    <row r="116" spans="1:40" s="20" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="18"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="17"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="17"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="18"/>
-      <c r="I116" s="18"/>
-      <c r="J116" s="22"/>
-      <c r="K116" s="18"/>
-      <c r="L116" s="29"/>
-      <c r="M116" s="24"/>
-      <c r="N116" s="18"/>
-      <c r="O116" s="18"/>
-      <c r="P116" s="18"/>
-      <c r="Q116" s="18"/>
-      <c r="R116" s="18"/>
-      <c r="S116" s="18"/>
-      <c r="T116" s="18"/>
-      <c r="U116" s="18"/>
-      <c r="V116" s="18"/>
-      <c r="W116" s="18"/>
-      <c r="X116" s="18"/>
-      <c r="Y116" s="18"/>
-      <c r="Z116" s="18"/>
-      <c r="AA116" s="18"/>
-      <c r="AB116" s="18"/>
-      <c r="AC116" s="18"/>
-      <c r="AD116" s="17"/>
-      <c r="AE116" s="18"/>
-      <c r="AF116" s="17"/>
-      <c r="AG116" s="17"/>
-      <c r="AH116" s="25"/>
-      <c r="AI116" s="17"/>
-      <c r="AJ116" s="17"/>
-      <c r="AK116" s="17"/>
-      <c r="AL116" s="26"/>
-      <c r="AM116" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN116" s="27"/>
-    </row>
-    <row r="117" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="20"/>
-      <c r="D117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="J117" s="22"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="24"/>
-      <c r="AD117" s="17"/>
-      <c r="AF117" s="17"/>
-      <c r="AG117" s="17"/>
-      <c r="AH117" s="25"/>
-      <c r="AI117" s="17"/>
-      <c r="AJ117" s="17"/>
-      <c r="AK117" s="17"/>
-      <c r="AL117" s="26"/>
-      <c r="AM117" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN117" s="27"/>
-    </row>
-    <row r="118" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="20"/>
-      <c r="D118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="J118" s="22"/>
-      <c r="L118" s="29"/>
-      <c r="M118" s="24"/>
-      <c r="AD118" s="17"/>
-      <c r="AF118" s="17"/>
-      <c r="AG118" s="17"/>
-      <c r="AH118" s="25"/>
-      <c r="AI118" s="17"/>
-      <c r="AJ118" s="17"/>
-      <c r="AK118" s="17"/>
-      <c r="AL118" s="26"/>
-      <c r="AM118" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN118" s="27"/>
-    </row>
-    <row r="119" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="20"/>
-      <c r="D119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="J119" s="22"/>
-      <c r="L119" s="29"/>
-      <c r="M119" s="24"/>
-      <c r="AD119" s="17"/>
-      <c r="AF119" s="17"/>
-      <c r="AG119" s="17"/>
-      <c r="AH119" s="25"/>
-      <c r="AI119" s="17"/>
-      <c r="AJ119" s="17"/>
-      <c r="AK119" s="17"/>
-      <c r="AL119" s="26"/>
-      <c r="AM119" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN119" s="27"/>
-    </row>
-    <row r="120" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="20"/>
-      <c r="D120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="J120" s="22"/>
-      <c r="L120" s="29"/>
-      <c r="M120" s="24"/>
-      <c r="AD120" s="17"/>
-      <c r="AF120" s="17"/>
-      <c r="AG120" s="17"/>
-      <c r="AH120" s="25"/>
-      <c r="AI120" s="17"/>
-      <c r="AJ120" s="17"/>
-      <c r="AK120" s="17"/>
-      <c r="AL120" s="26"/>
-      <c r="AM120" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN120" s="27"/>
-    </row>
-    <row r="121" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="20"/>
-      <c r="D121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="J121" s="22"/>
-      <c r="L121" s="29"/>
-      <c r="M121" s="24"/>
-      <c r="AD121" s="17"/>
-      <c r="AF121" s="17"/>
-      <c r="AG121" s="17"/>
-      <c r="AH121" s="25"/>
-      <c r="AI121" s="17"/>
-      <c r="AJ121" s="17"/>
-      <c r="AK121" s="17"/>
-      <c r="AL121" s="26"/>
-      <c r="AM121" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN121" s="27"/>
-    </row>
-    <row r="122" spans="1:40" s="18" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="20"/>
-      <c r="D122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="J122" s="22"/>
-      <c r="L122" s="29"/>
-      <c r="M122" s="24"/>
-      <c r="AD122" s="17"/>
-      <c r="AF122" s="17"/>
-      <c r="AG122" s="17"/>
-      <c r="AH122" s="25"/>
-      <c r="AI122" s="17"/>
-      <c r="AJ122" s="17"/>
-      <c r="AK122" s="17"/>
-      <c r="AL122" s="26"/>
-      <c r="AM122" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN122" s="27"/>
-    </row>
-    <row r="123" spans="1:40" s="18" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="20"/>
-      <c r="D123" s="17"/>
-      <c r="F123" s="17"/>
-      <c r="J123" s="22"/>
-      <c r="L123" s="29"/>
-      <c r="M123" s="24"/>
-      <c r="AD123" s="17"/>
-      <c r="AF123" s="17"/>
-      <c r="AG123" s="17"/>
-      <c r="AH123" s="25"/>
-      <c r="AI123" s="17"/>
-      <c r="AJ123" s="17"/>
-      <c r="AK123" s="17"/>
-      <c r="AL123" s="26"/>
-      <c r="AM123" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN123" s="27"/>
-    </row>
-    <row r="124" spans="1:40" s="18" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="20"/>
-      <c r="D124" s="17"/>
-      <c r="F124" s="17"/>
-      <c r="J124" s="22"/>
-      <c r="L124" s="29"/>
-      <c r="M124" s="24"/>
-      <c r="AD124" s="17"/>
-      <c r="AF124" s="17"/>
-      <c r="AG124" s="17"/>
-      <c r="AH124" s="25"/>
-      <c r="AI124" s="17"/>
-      <c r="AJ124" s="17"/>
-      <c r="AK124" s="17"/>
-      <c r="AL124" s="26"/>
-      <c r="AM124" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN124" s="27"/>
-    </row>
-    <row r="125" spans="1:40" s="18" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="20"/>
-      <c r="D125" s="17"/>
-      <c r="F125" s="17"/>
-      <c r="J125" s="22"/>
-      <c r="L125" s="29"/>
-      <c r="M125" s="24"/>
-      <c r="AD125" s="17"/>
-      <c r="AF125" s="17"/>
-      <c r="AG125" s="17"/>
-      <c r="AH125" s="25"/>
-      <c r="AI125" s="17"/>
-      <c r="AJ125" s="17"/>
-      <c r="AK125" s="17"/>
-      <c r="AL125" s="26"/>
-      <c r="AM125" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="AN125" s="27"/>
+      <c r="AM29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:AN139" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AN43" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>